<commit_message>
2016-10-28:     1. 收盘总结 -26.90
</commit_message>
<xml_diff>
--- a/Stocks Info.xlsx
+++ b/Stocks Info.xlsx
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1694,12 +1694,12 @@
         <f>(D2-F2)/D2</f>
         <v>0.4904789494013132</v>
       </c>
-      <c r="I2" s="2">
-        <v>3113.22</v>
+      <c r="I2">
+        <v>3104.27</v>
       </c>
       <c r="J2" s="27">
         <f>(I2-F2)/(D2-F2)</f>
-        <v>0.1869984643855572</v>
+        <v>0.1834744261133204</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>125</v>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="Q2" s="2">
         <f>SUM(Q3:Q42)</f>
-        <v>7137</v>
+        <v>7133</v>
       </c>
       <c r="R2" s="2"/>
       <c r="S2" s="2">
@@ -1744,7 +1744,7 @@
         <f>(D3-F3)/D3</f>
         <v>0.32659932659932667</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3">
         <v>4.4400000000000004</v>
       </c>
       <c r="J3" s="27">
@@ -1802,12 +1802,12 @@
         <f t="shared" ref="H4:H42" si="0">(D4-F4)/D4</f>
         <v>6.6869300911854168E-2</v>
       </c>
-      <c r="I4" s="2">
-        <v>3.16</v>
+      <c r="I4">
+        <v>3.17</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ref="J4:J41" si="1">(I4-F4)/(D4-F4)</f>
-        <v>0.40909090909091012</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="K4">
         <v>5</v>
@@ -1857,12 +1857,12 @@
         <f t="shared" si="0"/>
         <v>7.9999999999999974E-2</v>
       </c>
-      <c r="I5" s="2">
-        <v>17.88</v>
+      <c r="I5">
+        <v>17.899999999999999</v>
       </c>
       <c r="J5" s="27">
         <f t="shared" si="1"/>
-        <v>0.26315789473684126</v>
+        <v>0.27631578947368307</v>
       </c>
       <c r="K5">
         <v>3</v>
@@ -1912,7 +1912,7 @@
         <f t="shared" si="0"/>
         <v>9.1210613598673274E-2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>5.65</v>
       </c>
       <c r="J6" s="28">
@@ -1967,12 +1967,12 @@
         <f t="shared" si="0"/>
         <v>7.5812274368231028E-2</v>
       </c>
-      <c r="I7" s="2">
-        <v>5.28</v>
+      <c r="I7">
+        <v>5.26</v>
       </c>
       <c r="J7" s="28">
         <f t="shared" si="1"/>
-        <v>0.38095238095238138</v>
+        <v>0.33333333333333265</v>
       </c>
       <c r="K7">
         <v>4</v>
@@ -2022,12 +2022,12 @@
         <f t="shared" si="0"/>
         <v>0.21029082774049229</v>
       </c>
-      <c r="I8" s="2">
-        <v>20.34</v>
+      <c r="I8">
+        <v>20.04</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" si="1"/>
-        <v>0.57234042553191478</v>
+        <v>0.50851063829787213</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -2077,12 +2077,12 @@
         <f t="shared" si="0"/>
         <v>0.12525150905432589</v>
       </c>
-      <c r="I9" s="2">
-        <v>17.96</v>
+      <c r="I9">
+        <v>17.920000000000002</v>
       </c>
       <c r="J9" s="27">
         <f t="shared" si="1"/>
-        <v>0.22891566265060267</v>
+        <v>0.21285140562249055</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="Q9" s="2">
         <f t="shared" si="3"/>
-        <v>1796</v>
+        <v>1792.0000000000002</v>
       </c>
       <c r="R9" s="2">
         <v>18.02</v>
@@ -2138,12 +2138,12 @@
         <f t="shared" si="0"/>
         <v>0.12310902451747537</v>
       </c>
-      <c r="I10" s="2">
-        <v>18.3</v>
+      <c r="I10">
+        <v>18.190000000000001</v>
       </c>
       <c r="J10" s="28">
         <f t="shared" si="1"/>
-        <v>0.63135593220338992</v>
+        <v>0.58474576271186474</v>
       </c>
       <c r="K10">
         <v>3</v>
@@ -2193,12 +2193,12 @@
         <f t="shared" si="0"/>
         <v>0.15417106652587126</v>
       </c>
-      <c r="I11" s="2">
-        <v>17.07</v>
+      <c r="I11">
+        <v>16.95</v>
       </c>
       <c r="J11" s="28">
         <f t="shared" si="1"/>
-        <v>0.35958904109589046</v>
+        <v>0.31849315068493123</v>
       </c>
       <c r="K11">
         <v>4</v>
@@ -2248,12 +2248,12 @@
         <f t="shared" si="0"/>
         <v>0.15064102564102558</v>
       </c>
-      <c r="I12" s="2">
-        <v>16.91</v>
+      <c r="I12">
+        <v>16.809999999999999</v>
       </c>
       <c r="J12" s="28">
         <f>(I12-F12)/(D12-F12)</f>
-        <v>0.35815602836879445</v>
+        <v>0.32269503546099249</v>
       </c>
       <c r="K12">
         <v>4</v>
@@ -2303,12 +2303,12 @@
         <f t="shared" si="0"/>
         <v>0.18533236994219648</v>
       </c>
-      <c r="I13" s="2">
-        <v>24.64</v>
+      <c r="I13">
+        <v>24.75</v>
       </c>
       <c r="J13" s="28">
         <f t="shared" si="1"/>
-        <v>0.40740740740740744</v>
+        <v>0.42884990253411298</v>
       </c>
       <c r="K13">
         <v>2</v>
@@ -2358,7 +2358,7 @@
         <f t="shared" si="0"/>
         <v>0.16188714153561518</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14">
         <v>9.17</v>
       </c>
       <c r="J14" s="27">
@@ -2422,12 +2422,12 @@
         <f t="shared" si="0"/>
         <v>0.12913117546848391</v>
       </c>
-      <c r="I15" s="2">
-        <v>27.52</v>
+      <c r="I15">
+        <v>27.32</v>
       </c>
       <c r="J15" s="28">
         <f t="shared" si="1"/>
-        <v>0.51715039577836397</v>
+        <v>0.46437994722955156</v>
       </c>
       <c r="K15">
         <v>4</v>
@@ -2477,12 +2477,12 @@
         <f t="shared" si="0"/>
         <v>0.11643835616438351</v>
       </c>
-      <c r="I16" s="2">
-        <v>16.88</v>
+      <c r="I16">
+        <v>16.79</v>
       </c>
       <c r="J16" s="28">
         <f t="shared" si="1"/>
-        <v>0.68627450980392113</v>
+        <v>0.64215686274509765</v>
       </c>
       <c r="K16">
         <v>3</v>
@@ -2532,12 +2532,12 @@
         <f t="shared" si="0"/>
         <v>0.15077319587628865</v>
       </c>
-      <c r="I17" s="2">
-        <v>7.01</v>
+      <c r="I17">
+        <v>6.95</v>
       </c>
       <c r="J17" s="28">
         <f t="shared" si="1"/>
-        <v>0.35897435897435892</v>
+        <v>0.30769230769230799</v>
       </c>
       <c r="K17">
         <v>3</v>
@@ -2587,12 +2587,12 @@
         <f t="shared" si="0"/>
         <v>0.12634309003334571</v>
       </c>
-      <c r="I18" s="2">
-        <v>24.83</v>
+      <c r="I18">
+        <v>24.91</v>
       </c>
       <c r="J18" s="28">
         <f t="shared" si="1"/>
-        <v>0.36656891495601174</v>
+        <v>0.39002932551319702</v>
       </c>
       <c r="K18">
         <v>3</v>
@@ -2642,12 +2642,12 @@
         <f t="shared" si="0"/>
         <v>0.20406976744186045</v>
       </c>
-      <c r="I19" s="2">
-        <v>14.17</v>
+      <c r="I19">
+        <v>14.23</v>
       </c>
       <c r="J19" s="27">
         <f t="shared" si="1"/>
-        <v>0.13675213675213688</v>
+        <v>0.15384615384615413</v>
       </c>
       <c r="K19">
         <v>4</v>
@@ -2697,12 +2697,12 @@
         <f t="shared" si="0"/>
         <v>7.5941289087428171E-2</v>
       </c>
-      <c r="I20" s="2">
-        <v>15.55</v>
+      <c r="I20">
+        <v>15.48</v>
       </c>
       <c r="J20" s="29">
         <f t="shared" si="1"/>
-        <v>0.8991596638655468</v>
+        <v>0.84033613445378186</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -2750,12 +2750,12 @@
         <f t="shared" si="0"/>
         <v>6.8994889267461709E-2</v>
       </c>
-      <c r="I21" s="2">
-        <v>22.39</v>
-      </c>
-      <c r="J21" s="28">
+      <c r="I21">
+        <v>22.3</v>
+      </c>
+      <c r="J21" s="27">
         <f t="shared" si="1"/>
-        <v>0.327160493827161</v>
+        <v>0.27160493827160553</v>
       </c>
       <c r="K21">
         <v>2</v>
@@ -2805,12 +2805,12 @@
         <f t="shared" si="0"/>
         <v>8.3601286173633452E-2</v>
       </c>
-      <c r="I22" s="2">
-        <v>21.3</v>
-      </c>
-      <c r="J22" s="28">
+      <c r="I22">
+        <v>21.55</v>
+      </c>
+      <c r="J22" s="29">
         <f t="shared" si="1"/>
-        <v>0.74175824175824245</v>
+        <v>0.87912087912087977</v>
       </c>
       <c r="K22">
         <v>2</v>
@@ -2860,12 +2860,12 @@
         <f t="shared" si="0"/>
         <v>0.17871006270528525</v>
       </c>
-      <c r="I23" s="2">
-        <v>59.66</v>
+      <c r="I23">
+        <v>59.24</v>
       </c>
       <c r="J23" s="28">
         <f t="shared" si="1"/>
-        <v>0.38847117794486186</v>
+        <v>0.35338345864661669</v>
       </c>
       <c r="K23">
         <v>3</v>
@@ -2915,12 +2915,12 @@
         <f t="shared" si="0"/>
         <v>0.10736975857687417</v>
       </c>
-      <c r="I24" s="2">
-        <v>30.14</v>
+      <c r="I24">
+        <v>29.91</v>
       </c>
       <c r="J24" s="28">
         <f t="shared" si="1"/>
-        <v>0.60355029585798814</v>
+        <v>0.53550295857988139</v>
       </c>
       <c r="K24">
         <v>4</v>
@@ -2970,12 +2970,12 @@
         <f t="shared" si="0"/>
         <v>0.19262917933130699</v>
       </c>
-      <c r="I25" s="2">
-        <v>22.7</v>
-      </c>
-      <c r="J25" s="27">
+      <c r="I25">
+        <v>22.92</v>
+      </c>
+      <c r="J25" s="28">
         <f t="shared" si="1"/>
-        <v>0.28599605522682431</v>
+        <v>0.32938856015779122</v>
       </c>
       <c r="K25">
         <v>2</v>
@@ -3025,12 +3025,12 @@
         <f t="shared" si="0"/>
         <v>0.27370304114490168</v>
       </c>
-      <c r="I26" s="2">
-        <v>5.15</v>
+      <c r="I26">
+        <v>5.13</v>
       </c>
       <c r="J26" s="29">
         <f t="shared" si="1"/>
-        <v>0.71241830065359513</v>
+        <v>0.69934640522875824</v>
       </c>
       <c r="K26">
         <v>5</v>
@@ -3080,12 +3080,12 @@
         <f t="shared" si="0"/>
         <v>0.1006036217303823</v>
       </c>
-      <c r="I27" s="2">
-        <v>9.5399999999999991</v>
+      <c r="I27">
+        <v>9.41</v>
       </c>
       <c r="J27" s="28">
         <f t="shared" si="1"/>
-        <v>0.59999999999999964</v>
+        <v>0.47000000000000064</v>
       </c>
       <c r="K27">
         <v>4</v>
@@ -3135,12 +3135,12 @@
         <f t="shared" si="0"/>
         <v>0.16915995397008055</v>
       </c>
-      <c r="I28" s="2">
-        <v>7.4</v>
+      <c r="I28">
+        <v>7.36</v>
       </c>
       <c r="J28" s="27">
         <f t="shared" si="1"/>
-        <v>0.12244897959183716</v>
+        <v>9.5238095238095635E-2</v>
       </c>
       <c r="K28">
         <v>3</v>
@@ -3190,7 +3190,7 @@
         <f t="shared" si="0"/>
         <v>0.23880597014925381</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29">
         <v>5.18</v>
       </c>
       <c r="J29" s="27">
@@ -3254,12 +3254,12 @@
         <f t="shared" si="0"/>
         <v>0.21885521885521886</v>
       </c>
-      <c r="I30" s="2">
-        <v>7.12</v>
+      <c r="I30">
+        <v>7.09</v>
       </c>
       <c r="J30" s="27">
         <f t="shared" si="1"/>
-        <v>8.2051282051282121E-2</v>
+        <v>6.666666666666661E-2</v>
       </c>
       <c r="K30">
         <v>4</v>
@@ -3309,12 +3309,12 @@
         <f t="shared" si="0"/>
         <v>9.4890510948905188E-2</v>
       </c>
-      <c r="I31" s="2">
-        <v>5.27</v>
+      <c r="I31">
+        <v>5.23</v>
       </c>
       <c r="J31" s="28">
         <f t="shared" si="1"/>
-        <v>0.59615384615384492</v>
+        <v>0.51923076923076961</v>
       </c>
       <c r="K31">
         <v>2</v>
@@ -3364,7 +3364,7 @@
         <f t="shared" si="0"/>
         <v>4.7745358090185722E-2</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32">
         <v>7.38</v>
       </c>
       <c r="J32" s="28">
@@ -3419,12 +3419,12 @@
         <f t="shared" si="0"/>
         <v>0.25761124121779855</v>
       </c>
-      <c r="I33" s="2">
-        <v>16.510000000000002</v>
+      <c r="I33">
+        <v>16.48</v>
       </c>
       <c r="J33" s="29">
         <f t="shared" si="1"/>
-        <v>0.87045454545454615</v>
+        <v>0.86363636363636409</v>
       </c>
       <c r="K33">
         <v>4</v>
@@ -3474,7 +3474,7 @@
         <f t="shared" si="0"/>
         <v>7.3929961089494151E-2</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34">
         <v>5.01</v>
       </c>
       <c r="J34" s="28">
@@ -3529,12 +3529,12 @@
         <f t="shared" si="0"/>
         <v>0.10814249363867691</v>
       </c>
-      <c r="I35" s="2">
-        <v>7.18</v>
+      <c r="I35">
+        <v>7.17</v>
       </c>
       <c r="J35" s="27">
         <f t="shared" si="1"/>
-        <v>0.19999999999999979</v>
+        <v>0.18823529411764711</v>
       </c>
       <c r="K35">
         <v>3</v>
@@ -3584,7 +3584,7 @@
         <f t="shared" si="0"/>
         <v>4.8387096774193519E-2</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36">
         <v>3.02</v>
       </c>
       <c r="J36" s="28">
@@ -3639,12 +3639,12 @@
         <f t="shared" si="0"/>
         <v>8.9903181189488285E-2</v>
       </c>
-      <c r="I37" s="2">
-        <v>6.84</v>
+      <c r="I37">
+        <v>6.8</v>
       </c>
       <c r="J37" s="28">
         <f t="shared" si="1"/>
-        <v>0.39999999999999947</v>
+        <v>0.33846153846153787</v>
       </c>
       <c r="K37">
         <v>3</v>
@@ -3694,12 +3694,12 @@
         <f t="shared" si="0"/>
         <v>0.20293609671848012</v>
       </c>
-      <c r="I38" s="2">
-        <v>19.48</v>
+      <c r="I38">
+        <v>19.309999999999999</v>
       </c>
       <c r="J38" s="27">
         <f t="shared" si="1"/>
-        <v>0.21702127659574463</v>
+        <v>0.1808510638297868</v>
       </c>
       <c r="K38">
         <v>3</v>
@@ -3749,12 +3749,12 @@
         <f t="shared" si="0"/>
         <v>0.19617321248741193</v>
       </c>
-      <c r="I39" s="2">
-        <v>44.2</v>
+      <c r="I39">
+        <v>43.34</v>
       </c>
       <c r="J39" s="28">
         <f t="shared" si="1"/>
-        <v>0.44045174537987736</v>
+        <v>0.35215605749486717</v>
       </c>
       <c r="K39">
         <v>3</v>
@@ -3802,12 +3802,12 @@
         <f t="shared" si="0"/>
         <v>0.1749333333333333</v>
       </c>
-      <c r="I40" s="2">
-        <v>31.92</v>
+      <c r="I40">
+        <v>31.69</v>
       </c>
       <c r="J40" s="27">
         <f t="shared" si="1"/>
-        <v>0.14939024390243913</v>
+        <v>0.11432926829268295</v>
       </c>
       <c r="K40">
         <v>3</v>
@@ -3857,12 +3857,12 @@
         <f t="shared" si="0"/>
         <v>0.1957273012880929</v>
       </c>
-      <c r="I41" s="2">
-        <v>26.98</v>
+      <c r="I41">
+        <v>26.87</v>
       </c>
       <c r="J41" s="27">
         <f t="shared" si="1"/>
-        <v>0.22150882825040125</v>
+        <v>0.2038523274478331</v>
       </c>
       <c r="K41">
         <v>3</v>
@@ -3910,12 +3910,12 @@
         <f t="shared" si="0"/>
         <v>0.19421172886519425</v>
       </c>
-      <c r="I42" s="2">
-        <v>23.33</v>
+      <c r="I42">
+        <v>23.24</v>
       </c>
       <c r="J42" s="28">
         <f>(I42-F42)/(D42-F42)</f>
-        <v>0.42549019607843092</v>
+        <v>0.40784313725490151</v>
       </c>
       <c r="K42">
         <v>3</v>

</xml_diff>